<commit_message>
Berhasil Kirim Laporan dan foto update tagsus
Berhasil Kirim Laporan dan foto update tagsus
</commit_message>
<xml_diff>
--- a/data/listuser/command.xlsx
+++ b/data/listuser/command.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\GitHub\NEWASMENTE\data\listuser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05002155-5317-4435-885F-7BB469FB5099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7566D516-0EF6-4CB5-B710-564ABF466767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{090BDAAA-3D4B-46BE-B3E8-44D57DE99DBA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{090BDAAA-3D4B-46BE-B3E8-44D57DE99DBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="26">
   <si>
     <t>a</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>v</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -469,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FFD962E-5CBC-44FA-ACD8-5B43AE5550AD}">
-  <dimension ref="C2:BA36"/>
+  <dimension ref="C2:BA40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="AH34" sqref="AH34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1984,7 +1987,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C33" s="1">
         <v>0</v>
       </c>
@@ -2016,7 +2019,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C35" s="1" t="s">
         <v>1</v>
       </c>
@@ -2048,7 +2051,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C36" s="1">
         <v>0</v>
       </c>
@@ -2077,6 +2080,91 @@
         <v>8</v>
       </c>
       <c r="L36" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J39" s="1">
+        <v>8</v>
+      </c>
+      <c r="K39" s="1">
+        <v>9</v>
+      </c>
+      <c r="L39" s="1">
+        <v>0</v>
+      </c>
+      <c r="M39" s="1">
+        <v>8</v>
+      </c>
+      <c r="N39" s="1">
+        <v>0</v>
+      </c>
+      <c r="O39" s="1">
+        <v>8</v>
+      </c>
+      <c r="P39" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q39" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S39" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C40" s="1">
+        <v>0</v>
+      </c>
+      <c r="D40" s="1">
+        <v>1</v>
+      </c>
+      <c r="E40" s="1">
+        <v>2</v>
+      </c>
+      <c r="F40" s="1">
+        <v>3</v>
+      </c>
+      <c r="G40" s="1">
+        <v>4</v>
+      </c>
+      <c r="H40" s="1">
+        <v>5</v>
+      </c>
+      <c r="I40" s="1">
+        <v>6</v>
+      </c>
+      <c r="J40" s="1">
+        <v>7</v>
+      </c>
+      <c r="K40" s="1">
+        <v>8</v>
+      </c>
+      <c r="L40" s="1">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Menghitung jumlah row dengan benar
Menghitung jumlah row pembelian token sudah benar, menggunakan metode cari element parentnya, dan hitung jumlah child elementnya
</commit_message>
<xml_diff>
--- a/data/listuser/command.xlsx
+++ b/data/listuser/command.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\GitHub\NEWASMENTE\data\listuser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7566D516-0EF6-4CB5-B710-564ABF466767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33C63F8-DCD3-46E8-9431-FDDDDBB0DDAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{090BDAAA-3D4B-46BE-B3E8-44D57DE99DBA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="26">
   <si>
     <t>a</t>
   </si>
@@ -472,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FFD962E-5CBC-44FA-ACD8-5B43AE5550AD}">
-  <dimension ref="C2:BA40"/>
+  <dimension ref="C2:BA43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="AH34" sqref="AH34"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="AD40" sqref="AD40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1987,7 +1987,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:24" x14ac:dyDescent="0.35">
       <c r="C33" s="1">
         <v>0</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:24" x14ac:dyDescent="0.35">
       <c r="C35" s="1" t="s">
         <v>1</v>
       </c>
@@ -2051,7 +2051,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:24" x14ac:dyDescent="0.35">
       <c r="C36" s="1">
         <v>0</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:24" x14ac:dyDescent="0.35">
       <c r="C39" s="1" t="s">
         <v>14</v>
       </c>
@@ -2136,7 +2136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:24" x14ac:dyDescent="0.35">
       <c r="C40" s="1">
         <v>0</v>
       </c>
@@ -2166,6 +2166,142 @@
       </c>
       <c r="L40" s="1">
         <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="C42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M42" s="1">
+        <v>3</v>
+      </c>
+      <c r="N42" s="1">
+        <v>2</v>
+      </c>
+      <c r="O42" s="1">
+        <v>1</v>
+      </c>
+      <c r="P42" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q42" s="1">
+        <v>0</v>
+      </c>
+      <c r="R42" s="1">
+        <v>0</v>
+      </c>
+      <c r="S42" s="1">
+        <v>7</v>
+      </c>
+      <c r="T42" s="1">
+        <v>6</v>
+      </c>
+      <c r="U42" s="1">
+        <v>5</v>
+      </c>
+      <c r="V42" s="1">
+        <v>4</v>
+      </c>
+      <c r="W42" s="1">
+        <v>3</v>
+      </c>
+      <c r="X42" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="C43" s="1">
+        <v>0</v>
+      </c>
+      <c r="D43" s="1">
+        <v>1</v>
+      </c>
+      <c r="E43" s="1">
+        <v>2</v>
+      </c>
+      <c r="F43" s="1">
+        <v>3</v>
+      </c>
+      <c r="G43" s="1">
+        <v>4</v>
+      </c>
+      <c r="H43" s="1">
+        <v>5</v>
+      </c>
+      <c r="I43" s="1">
+        <v>6</v>
+      </c>
+      <c r="J43" s="1">
+        <v>7</v>
+      </c>
+      <c r="K43" s="1">
+        <v>8</v>
+      </c>
+      <c r="L43" s="1">
+        <v>9</v>
+      </c>
+      <c r="M43" s="1">
+        <v>10</v>
+      </c>
+      <c r="N43" s="1">
+        <v>11</v>
+      </c>
+      <c r="O43" s="1">
+        <v>12</v>
+      </c>
+      <c r="P43" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q43" s="1">
+        <v>14</v>
+      </c>
+      <c r="R43" s="1">
+        <v>15</v>
+      </c>
+      <c r="S43" s="1">
+        <v>16</v>
+      </c>
+      <c r="T43" s="1">
+        <v>17</v>
+      </c>
+      <c r="U43" s="1">
+        <v>18</v>
+      </c>
+      <c r="V43" s="1">
+        <v>19</v>
+      </c>
+      <c r="W43" s="1">
+        <v>20</v>
+      </c>
+      <c r="X43" s="1">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>